<commit_message>
801623 Added Text to empty Defect Log indicating that no defects were found
</commit_message>
<xml_diff>
--- a/TASCore_documents/Test/Build 5/TAS_Core_Defect_Log_TAS.01.00.1453_20180824_134457.xlsx
+++ b/TASCore_documents/Test/Build 5/TAS_Core_Defect_Log_TAS.01.00.1453_20180824_134457.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VHAISPBRUNOL\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vhaisathompv\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19695" windowHeight="7155" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Department of Veterans Affairs</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Lisa Bruno/Donald Fowlds</t>
+  </si>
+  <si>
+    <t>NO DEFECTS WERE FOUND</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,12 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -413,14 +421,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1008,7 +1011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:H3"/>
     </sheetView>
   </sheetViews>
@@ -1034,28 +1037,28 @@
       <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="14"/>
@@ -1094,28 +1097,28 @@
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
@@ -1170,12 +1173,12 @@
       <c r="A1" s="3"/>
     </row>
     <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -1234,11 +1237,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:J2"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,6 +1292,11 @@
         <v>18</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J14"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>